<commit_message>
Contact export method implemented
</commit_message>
<xml_diff>
--- a/Contact/src/main/resources/contact.xlsx
+++ b/Contact/src/main/resources/contact.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28004"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,21 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,65 +47,65 @@
     <t>email</t>
   </si>
   <si>
+    <t>dob</t>
+  </si>
+  <si>
     <t>mobile</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
     <t>Sam</t>
   </si>
   <si>
+    <t>sam@gmail.com</t>
+  </si>
+  <si>
     <t>Ram</t>
   </si>
   <si>
+    <t>ram123@gmail.com</t>
+  </si>
+  <si>
     <t>Tom</t>
   </si>
   <si>
+    <t>tom45@yahoo.com</t>
+  </si>
+  <si>
     <t>Jill</t>
   </si>
   <si>
+    <t>jill18@gmail.com</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
+    <t>johnson@gmail.com</t>
+  </si>
+  <si>
     <t>James</t>
   </si>
   <si>
+    <t>james91@yahoo.com</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>william@gmail.com</t>
+  </si>
+  <si>
     <t>Vijay</t>
   </si>
   <si>
-    <t>sam@gmail.com</t>
-  </si>
-  <si>
     <t>vijay@gmail.com</t>
-  </si>
-  <si>
-    <t>ram123@gmail.com</t>
-  </si>
-  <si>
-    <t>tom45@yahoo.com</t>
-  </si>
-  <si>
-    <t>jill18@gmail.com</t>
-  </si>
-  <si>
-    <t>johnson@gmail.com</t>
-  </si>
-  <si>
-    <t>james91@yahoo.com</t>
-  </si>
-  <si>
-    <t>Will</t>
-  </si>
-  <si>
-    <t>william@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,14 +434,14 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,13 +452,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -455,7 +466,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
         <v>35903</v>
@@ -464,15 +475,15 @@
         <v>5432109876</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>36269</v>
@@ -481,15 +492,15 @@
         <v>2345167890</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>37598</v>
@@ -498,15 +509,15 @@
         <v>4321987650</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>38380</v>
@@ -515,15 +526,15 @@
         <v>9087654321</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2">
         <v>36386</v>
@@ -532,15 +543,15 @@
         <v>9980765342</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
         <v>36934</v>
@@ -549,15 +560,15 @@
         <v>3124586790</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2">
         <v>36060</v>
@@ -566,15 +577,15 @@
         <v>7612345908</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2">
         <v>35387</v>

</xml_diff>